<commit_message>
fixed to take into account duplicate entries in the nova.compute_nodes table
</commit_message>
<xml_diff>
--- a/capacity-report.xlsx
+++ b/capacity-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/migu4903/Documents/RPC/osa-capacity-report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40639970-51DA-2446-AE91-E126FA23C579}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB08A668-4F93-274B-88A2-BF2F78CD8926}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="580" windowWidth="34380" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="460" windowWidth="34380" windowHeight="17700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="DATA" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="bcus_perf_1" localSheetId="2">DATA!$A$2:$W$5</definedName>
     <definedName name="DATES" localSheetId="2">OFFSET(DATA!$A$1,1,0,COUNTA(DATA!$A:$A)-1,1)</definedName>
     <definedName name="DATES">OFFSET(DATA!$A$1,1,0,COUNTA(DATA!$A:$A)-1,1)</definedName>
     <definedName name="DEV_CPU_PERC">OFFSET([0]!DEV_DATES,0,20)</definedName>
@@ -51,40 +50,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{CD0A1434-EE55-E340-8609-66E1D9F5B1BE}" name="bcus-perf1" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr prompt="0" sourceFile="/Users/migu4903/OneDrive - Rackspace Inc/capacity-reports/bcus-perf.csv" tab="0" semicolon="1">
-      <textFields count="23">
-        <textField type="YMD"/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,18 +424,9 @@
               <c:f>DATA!DATES</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>43514</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43539</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43542</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43543</c:v>
+                  <c:v>43553</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -480,18 +436,9 @@
               <c:f>DATA!PERF_VMS</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>313</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>331</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>331</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>467</c:v>
+                  <c:v>469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -790,18 +737,9 @@
               <c:f>DATA!DATES</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>43514</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43539</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43542</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43543</c:v>
+                  <c:v>43553</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -810,19 +748,10 @@
             <c:numRef>
               <c:f>[0]!PERF_MEM_PERC</c:f>
               <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0" formatCode="0.0000">
-                  <c:v>0.39200000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.40710000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>0.40710200000000002</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>0.51957500000000001</c:v>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.448876</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -869,18 +798,9 @@
               <c:f>DATA!DATES</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>43514</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43539</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43542</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43543</c:v>
+                  <c:v>43553</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -889,19 +809,10 @@
             <c:numRef>
               <c:f>[0]!PERF_CPU_PERC</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0" formatCode="0.0000">
-                  <c:v>0.33210000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.33900000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.343333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.47</c:v>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.41206399999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -948,18 +859,9 @@
               <c:f>DATA!DATES</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>43514</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43539</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43542</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43543</c:v>
+                  <c:v>43553</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -968,19 +870,10 @@
             <c:numRef>
               <c:f>[0]!PERF_DISK_PERC</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0" formatCode="0.0000">
-                  <c:v>0.39369999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.41</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.40917999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.51993900000000004</c:v>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.44850499999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2359,10 +2252,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="bcus-perf_1" connectionId="1" xr16:uid="{BF917C87-A5EC-274E-911E-BBA374DB8B9E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2663,7 +2552,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -2717,7 +2606,7 @@
       </c>
       <c r="B7" s="1">
         <f ca="1">OFFSET(DATA!A1,COUNTA(DATA!$A:$A)-1,0)</f>
-        <v>43543</v>
+        <v>43553</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2735,7 +2624,7 @@
       </c>
       <c r="B9">
         <f ca="1">OFFSET(DATA!C1,COUNTA(DATA!$C:$C)-1,0)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2744,7 +2633,7 @@
       </c>
       <c r="B10">
         <f ca="1">OFFSET(DATA!D1,COUNTA(DATA!$D:$D)-1,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2753,7 +2642,7 @@
       </c>
       <c r="B12">
         <f ca="1">OFFSET(DATA!E1,COUNTA(DATA!$E:$E)-1,0)</f>
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2762,7 +2651,7 @@
       </c>
       <c r="B14" s="5">
         <f ca="1">OFFSET(DATA!F1,COUNTA(DATA!$F:$F)-1,0)/1024</f>
-        <v>4026.984375</v>
+        <v>4027.0166015625</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2771,7 +2660,7 @@
       </c>
       <c r="B15" s="5">
         <f ca="1">OFFSET(DATA!G1,COUNTA(DATA!$G:$G)-1,0)/1024</f>
-        <v>755.0810546875</v>
+        <v>251.6630859375</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2780,7 +2669,7 @@
       </c>
       <c r="B16" s="5">
         <f ca="1">OFFSET(DATA!H1,COUNTA(DATA!$H:$H)-1,0)/1024</f>
-        <v>3271.9033203125</v>
+        <v>3775.353515625</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2789,7 +2678,7 @@
       </c>
       <c r="B17" s="6">
         <f ca="1">OFFSET(DATA!I1,COUNTA(DATA!$I:$I)-1,0)/1024</f>
-        <v>2550</v>
+        <v>2542</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="48" x14ac:dyDescent="0.2">
@@ -2798,7 +2687,7 @@
       </c>
       <c r="B18" s="7">
         <f ca="1">OFFSET(DATA!R1,COUNTA(DATA!$R:$R)-1,0)</f>
-        <v>0.42215200000000003</v>
+        <v>0.42082399999999998</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="80" x14ac:dyDescent="0.2">
@@ -2807,7 +2696,7 @@
       </c>
       <c r="B19" s="7">
         <f ca="1">OFFSET(DATA!S1,COUNTA(DATA!$S:$S)-1,0)</f>
-        <v>0.51957500000000001</v>
+        <v>0.448876</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2825,7 +2714,7 @@
       </c>
       <c r="B22">
         <f ca="1">OFFSET(DATA!K1,COUNTA(DATA!$K:$K)-1,0)</f>
-        <v>136</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2834,7 +2723,7 @@
       </c>
       <c r="B23">
         <f ca="1">OFFSET(DATA!L1,COUNTA(DATA!$L:$L)-1,0)</f>
-        <v>600</v>
+        <v>688</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2843,7 +2732,7 @@
       </c>
       <c r="B24">
         <f ca="1">OFFSET(DATA!M1,COUNTA(DATA!$M:$M)-1,0)</f>
-        <v>1128</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="48" x14ac:dyDescent="0.2">
@@ -2852,7 +2741,7 @@
       </c>
       <c r="B25" s="7">
         <f ca="1">OFFSET(DATA!T1,COUNTA(DATA!$T:$T)-1,0)</f>
-        <v>0.38315199999999999</v>
+        <v>0.38518999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="80" x14ac:dyDescent="0.2">
@@ -2861,7 +2750,7 @@
       </c>
       <c r="B26" s="7">
         <f ca="1">OFFSET(DATA!U1,COUNTA(DATA!$U:$U)-1,0)</f>
-        <v>0.47</v>
+        <v>0.41206399999999999</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -2879,7 +2768,7 @@
       </c>
       <c r="B29">
         <f ca="1">OFFSET(DATA!O1,COUNTA(DATA!$O:$O)-1,0)</f>
-        <v>11001</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2888,7 +2777,7 @@
       </c>
       <c r="B30">
         <f ca="1">OFFSET(DATA!P1,COUNTA(DATA!$P:$P)-1,0)</f>
-        <v>47671</v>
+        <v>55005</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2897,7 +2786,7 @@
       </c>
       <c r="B31">
         <f ca="1">OFFSET(DATA!Q1,COUNTA(DATA!$Q:$Q)-1,0)</f>
-        <v>24786</v>
+        <v>24670</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="48" x14ac:dyDescent="0.2">
@@ -2906,7 +2795,7 @@
       </c>
       <c r="B32" s="7">
         <f ca="1">OFFSET(DATA!V1,COUNTA(DATA!$V:$V)-1,0)</f>
-        <v>0.42244999999999999</v>
+        <v>0.42047299999999999</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -2915,7 +2804,7 @@
       </c>
       <c r="B33" s="7">
         <f ca="1">OFFSET(DATA!W1,COUNTA(DATA!$W:$W)-1,0)</f>
-        <v>0.51993900000000004</v>
+        <v>0.44850499999999999</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -2952,8 +2841,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3044,287 +2933,85 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43514</v>
+        <v>43553</v>
       </c>
       <c r="B2">
         <v>16</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>313</v>
+        <v>469</v>
       </c>
       <c r="F2">
-        <v>4123632</v>
+        <v>4123665</v>
       </c>
       <c r="G2">
-        <v>773203</v>
+        <v>257703</v>
       </c>
       <c r="H2">
-        <v>3350429</v>
+        <v>3865962</v>
       </c>
       <c r="I2">
-        <v>1970176</v>
+        <v>2603008</v>
       </c>
       <c r="J2">
         <v>736</v>
       </c>
       <c r="K2">
-        <v>136</v>
+        <v>48</v>
       </c>
       <c r="L2">
-        <v>600</v>
+        <v>688</v>
       </c>
       <c r="M2">
-        <v>797</v>
+        <v>1134</v>
       </c>
       <c r="N2">
         <v>58672</v>
       </c>
       <c r="O2">
-        <v>11001</v>
+        <v>3667</v>
       </c>
       <c r="P2">
-        <v>47671</v>
+        <v>55005</v>
       </c>
       <c r="Q2">
-        <v>18766</v>
+        <v>24670</v>
       </c>
       <c r="R2" s="8">
-        <v>0.31850000000000001</v>
+        <v>0.42082399999999998</v>
       </c>
       <c r="S2" s="8">
-        <v>0.39200000000000002</v>
+        <v>0.448876</v>
       </c>
       <c r="T2" s="8">
-        <v>0.2707</v>
+        <v>0.38518999999999998</v>
       </c>
       <c r="U2" s="8">
-        <v>0.33210000000000001</v>
+        <v>0.41206399999999999</v>
       </c>
       <c r="V2" s="8">
-        <v>0.31979999999999997</v>
+        <v>0.42047299999999999</v>
       </c>
       <c r="W2" s="8">
-        <v>0.39369999999999999</v>
+        <v>0.44850499999999999</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>43539</v>
-      </c>
-      <c r="B3">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>331</v>
-      </c>
-      <c r="F3">
-        <v>4123632</v>
-      </c>
-      <c r="G3">
-        <v>773203</v>
-      </c>
-      <c r="H3">
-        <v>3350429</v>
-      </c>
-      <c r="I3">
-        <v>2045952</v>
-      </c>
-      <c r="J3">
-        <v>736</v>
-      </c>
-      <c r="K3">
-        <v>136</v>
-      </c>
-      <c r="L3">
-        <v>600</v>
-      </c>
-      <c r="M3">
-        <v>824</v>
-      </c>
-      <c r="N3">
-        <v>58672</v>
-      </c>
-      <c r="O3">
-        <v>11001</v>
-      </c>
-      <c r="P3">
-        <v>47671</v>
-      </c>
-      <c r="Q3">
-        <v>19506</v>
-      </c>
-      <c r="R3" s="9">
-        <v>0.33077000000000001</v>
-      </c>
-      <c r="S3" s="9">
-        <v>0.40710000000000002</v>
-      </c>
-      <c r="T3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="U3">
-        <v>0.33900000000000002</v>
-      </c>
-      <c r="V3">
-        <v>0.33</v>
-      </c>
-      <c r="W3">
-        <v>0.41</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>43542</v>
-      </c>
-      <c r="B4">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>331</v>
-      </c>
-      <c r="F4">
-        <v>4123632</v>
-      </c>
-      <c r="G4">
-        <v>773203</v>
-      </c>
-      <c r="H4">
-        <v>3350429</v>
-      </c>
-      <c r="I4">
-        <v>2045952</v>
-      </c>
-      <c r="J4">
-        <v>736</v>
-      </c>
-      <c r="K4">
-        <v>136</v>
-      </c>
-      <c r="L4">
-        <v>600</v>
-      </c>
-      <c r="M4">
-        <v>824</v>
-      </c>
-      <c r="N4">
-        <v>58672</v>
-      </c>
-      <c r="O4">
-        <v>11001</v>
-      </c>
-      <c r="P4">
-        <v>47671</v>
-      </c>
-      <c r="Q4">
-        <v>19506</v>
-      </c>
-      <c r="R4">
-        <v>0.33076899999999998</v>
-      </c>
-      <c r="S4">
-        <v>0.40710200000000002</v>
-      </c>
-      <c r="T4">
-        <v>0.279891</v>
-      </c>
-      <c r="U4">
-        <v>0.343333</v>
-      </c>
-      <c r="V4">
-        <v>0.33245799999999998</v>
-      </c>
-      <c r="W4">
-        <v>0.40917999999999999</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>43543</v>
-      </c>
-      <c r="B5">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>467</v>
-      </c>
-      <c r="F5">
-        <v>4123632</v>
-      </c>
-      <c r="G5">
-        <v>773203</v>
-      </c>
-      <c r="H5">
-        <v>3350429</v>
-      </c>
-      <c r="I5">
-        <v>2611200</v>
-      </c>
-      <c r="J5">
-        <v>736</v>
-      </c>
-      <c r="K5">
-        <v>136</v>
-      </c>
-      <c r="L5">
-        <v>600</v>
-      </c>
-      <c r="M5">
-        <v>1128</v>
-      </c>
-      <c r="N5">
-        <v>58672</v>
-      </c>
-      <c r="O5">
-        <v>11001</v>
-      </c>
-      <c r="P5">
-        <v>47671</v>
-      </c>
-      <c r="Q5">
-        <v>24786</v>
-      </c>
-      <c r="R5">
-        <v>0.42215200000000003</v>
-      </c>
-      <c r="S5">
-        <v>0.51957500000000001</v>
-      </c>
-      <c r="T5">
-        <v>0.38315199999999999</v>
-      </c>
-      <c r="U5">
-        <v>0.47</v>
-      </c>
-      <c r="V5">
-        <v>0.42244999999999999</v>
-      </c>
-      <c r="W5">
-        <v>0.51993900000000004</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>